<commit_message>
v 1.04 implements structural addition of parallax sections
</commit_message>
<xml_diff>
--- a/portfolio-bootstrap/portfolio-bootstrap/font-analysis.xlsx
+++ b/portfolio-bootstrap/portfolio-bootstrap/font-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Web Dev\danzhaas.github.io\portfolio-bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D619107-80EC-45F4-87D2-7279094A65EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124D24B9-E3C0-41BB-8961-35CE3983BF44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11880" yWindow="4500" windowWidth="21600" windowHeight="11388" xr2:uid="{4F4F1B5B-DA29-414F-934A-72E6BC021AC5}"/>
+    <workbookView xWindow="-11880" yWindow="1092" windowWidth="21600" windowHeight="11388" xr2:uid="{4F4F1B5B-DA29-414F-934A-72E6BC021AC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="91">
   <si>
     <t>LANDING</t>
   </si>
@@ -248,6 +248,63 @@
   </si>
   <si>
     <t>cut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.navbar-brand </t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">.display-3   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">h5   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">.badge    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">body </t>
+  </si>
+  <si>
+    <t xml:space="preserve">.btn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#     max-width:   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">.fa-7x    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">body  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">p     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">body    </t>
+  </si>
+  <si>
+    <t>Changes2</t>
+  </si>
+  <si>
+    <t>small or good</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.contact-text  </t>
   </si>
 </sst>
 </file>
@@ -482,12 +539,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -497,11 +548,29 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -582,26 +651,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{308D8998-A54D-466C-8B5F-A0A41AE98DE1}" name="Table1" displayName="Table1" ref="A2:N22" totalsRowShown="0">
-  <autoFilter ref="A2:N22" xr:uid="{ED307D08-98E8-4842-A07F-C134845D7902}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{308D8998-A54D-466C-8B5F-A0A41AE98DE1}" name="Table1" displayName="Table1" ref="A2:O22" totalsRowShown="0">
+  <autoFilter ref="A2:O22" xr:uid="{ED307D08-98E8-4842-A07F-C134845D7902}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N22">
     <sortCondition ref="A2:A22"/>
   </sortState>
-  <tableColumns count="14">
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{3A9C98BE-0109-42FB-8BB4-10A44E726EF3}" name="Arrangement"/>
     <tableColumn id="9" xr3:uid="{B97A8DAB-F51D-41FA-B3D6-06B373BCDF3D}" name="Section"/>
-    <tableColumn id="2" xr3:uid="{F2C4E4F9-BA67-4306-8E40-7C3644B78F1C}" name="Elements" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F2C4E4F9-BA67-4306-8E40-7C3644B78F1C}" name="Elements" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{97034C5E-0468-4431-92C4-D53DFCDEA44D}" name="XS  font-size"/>
-    <tableColumn id="10" xr3:uid="{E60609C7-17F9-4FD6-9C2B-DBB60B1F4A02}" name="XS Rating" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{018873E3-3D96-4220-807B-8F6AB261B775}" name="Changes" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{E60609C7-17F9-4FD6-9C2B-DBB60B1F4A02}" name="XS Rating" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{018873E3-3D96-4220-807B-8F6AB261B775}" name="Changes" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{5B772071-8DAA-4340-BBF9-87EAF1175AFA}" name="SM  font-size"/>
-    <tableColumn id="11" xr3:uid="{60A0224E-AF8F-4BB6-B583-B5063A5B091B}" name="SM rating" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{60A0224E-AF8F-4BB6-B583-B5063A5B091B}" name="SM rating" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{90774B36-A071-4790-8308-284B405CDC37}" name="MD  font-size"/>
-    <tableColumn id="12" xr3:uid="{0CB73393-C792-425F-BD4A-A480C0A5B74E}" name="MD rating" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{0CB73393-C792-425F-BD4A-A480C0A5B74E}" name="MD rating" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{0BEA8A3F-B173-465C-9CF6-8832B4BDD53E}" name="LG  font-size"/>
-    <tableColumn id="13" xr3:uid="{F764AB20-BCBF-4C5C-9E1D-B6F03C66203C}" name="LG Rating" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{F764AB20-BCBF-4C5C-9E1D-B6F03C66203C}" name="LG Rating" dataDxfId="2"/>
     <tableColumn id="14" xr3:uid="{4D2D5282-B710-4D68-920A-DDE19EC9F2C7}" name="XL  font-size"/>
-    <tableColumn id="7" xr3:uid="{4DF0E1AD-3B18-4BBC-86E8-8FC7A967646A}" name="XL rating" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{4DF0E1AD-3B18-4BBC-86E8-8FC7A967646A}" name="XL rating" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{2B7C481B-116A-46B1-BCB8-F9E3A975CA35}" name="Changes2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -904,47 +974,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003AA83B-CD74-47A3-B603-85401DD0308B}">
-  <dimension ref="A1:N80"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="6" customWidth="1"/>
+    <col min="1" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="17"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -987,8 +1063,11 @@
       <c r="N2" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1007,16 +1086,27 @@
       <c r="F3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="J3" s="6"/>
-      <c r="K3" s="5"/>
+      <c r="K3" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="L3" s="6"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -1035,16 +1125,27 @@
       <c r="F4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="H4" s="8"/>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="J4" s="8"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="L4" s="8"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="8"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -1063,16 +1164,27 @@
       <c r="F5" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="H5" s="10"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="L5" s="10"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="10"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1091,16 +1203,27 @@
       <c r="F6" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="5"/>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="5"/>
+      <c r="K6" t="s">
+        <v>73</v>
+      </c>
       <c r="L6" s="6"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -1119,16 +1242,27 @@
       <c r="F7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="H7" s="8"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="J7" s="8"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="L7" s="8"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1162,9 +1296,12 @@
       <c r="M8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" s="11"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1183,16 +1320,27 @@
       <c r="F9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="J9" s="6"/>
-      <c r="K9" s="5"/>
+      <c r="K9" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="L9" s="6"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1211,16 +1359,27 @@
       <c r="F10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="J10" s="6"/>
-      <c r="K10" s="5"/>
+      <c r="K10" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="L10" s="6"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>8.5</v>
       </c>
@@ -1239,16 +1398,27 @@
       <c r="F11" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="J11" s="6"/>
-      <c r="K11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="L11" s="6"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -1267,16 +1437,27 @@
       <c r="F12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="H12" s="6"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="J12" s="6"/>
-      <c r="K12" s="5"/>
+      <c r="K12" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="L12" s="6"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -1295,16 +1476,27 @@
       <c r="F13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="H13" s="8"/>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="J13" s="8"/>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="L13" s="8"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -1338,9 +1530,12 @@
       <c r="M14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>12</v>
       </c>
@@ -1359,16 +1554,27 @@
       <c r="F15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="J15" s="6"/>
-      <c r="K15" s="5"/>
+      <c r="K15" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="L15" s="6"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M15" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>13</v>
       </c>
@@ -1387,16 +1593,27 @@
       <c r="F16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="J16" s="6"/>
-      <c r="K16" s="5"/>
+      <c r="K16" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="L16" s="6"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>14</v>
       </c>
@@ -1415,16 +1632,27 @@
       <c r="F17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="J17" s="6"/>
-      <c r="K17" s="5"/>
+      <c r="K17" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="L17" s="6"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="6"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -1443,16 +1671,27 @@
       <c r="F18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="J18" s="8"/>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="L18" s="8"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="8"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O18" s="8"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>16</v>
       </c>
@@ -1484,9 +1723,12 @@
       <c r="M19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>17</v>
       </c>
@@ -1505,16 +1747,27 @@
       <c r="F20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H20" s="6"/>
-      <c r="I20" s="5"/>
+      <c r="I20" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="J20" s="6"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="L20" s="6"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="6"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>18</v>
       </c>
@@ -1533,16 +1786,27 @@
       <c r="F21" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="H21" s="6"/>
-      <c r="I21" s="5"/>
+      <c r="I21" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="J21" s="6"/>
-      <c r="K21" s="5"/>
+      <c r="K21" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="L21" s="6"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="6"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M21" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>19</v>
       </c>
@@ -1561,70 +1825,81 @@
       <c r="F22" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="H22" s="8"/>
-      <c r="I22" s="1"/>
+      <c r="I22" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="J22" s="8"/>
-      <c r="K22" s="1"/>
+      <c r="K22" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="L22" s="8"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="8"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="5"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -1920,8 +2195,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D1:N1"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:O1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v 1.06 LAYOUT optimized for viewports down to ~350px; DESIGN improvements to navbar, added animations to showcase and about, re-drafted space-icon buttons
</commit_message>
<xml_diff>
--- a/portfolio-bootstrap/portfolio-bootstrap/font-analysis.xlsx
+++ b/portfolio-bootstrap/portfolio-bootstrap/font-analysis.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Web Dev\danzhaas.github.io\portfolio-bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124D24B9-E3C0-41BB-8961-35CE3983BF44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD6AEB0-BAB7-4B03-9861-F73C2CBC7A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11880" yWindow="1092" windowWidth="21600" windowHeight="11388" xr2:uid="{4F4F1B5B-DA29-414F-934A-72E6BC021AC5}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F4F1B5B-DA29-414F-934A-72E6BC021AC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="105">
   <si>
     <t>LANDING</t>
   </si>
@@ -139,9 +140,6 @@
     <t>XS Rating</t>
   </si>
   <si>
-    <t>SM rating</t>
-  </si>
-  <si>
     <t>XS  font-size</t>
   </si>
   <si>
@@ -214,9 +212,6 @@
     <t>too big</t>
   </si>
   <si>
-    <t>Changes</t>
-  </si>
-  <si>
     <t>#     max-width:   50vw</t>
   </si>
   <si>
@@ -305,6 +300,54 @@
   </si>
   <si>
     <t xml:space="preserve">.contact-text  </t>
+  </si>
+  <si>
+    <t>XS Changes</t>
+  </si>
+  <si>
+    <t>SM Changes</t>
+  </si>
+  <si>
+    <t>SM Rating</t>
+  </si>
+  <si>
+    <t>.navbar-brand 1.5rem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.display-4  </t>
+  </si>
+  <si>
+    <t>h2 4rem</t>
+  </si>
+  <si>
+    <t>h2   rem</t>
+  </si>
+  <si>
+    <t>.badge    1.25rem%</t>
+  </si>
+  <si>
+    <t>.btn 1.5 rem</t>
+  </si>
+  <si>
+    <t>#     max-width:   40vw</t>
+  </si>
+  <si>
+    <t>good big</t>
+  </si>
+  <si>
+    <t>can't see.  Probably too big</t>
+  </si>
+  <si>
+    <t>Squished</t>
+  </si>
+  <si>
+    <t>out-of-shape - too tall</t>
+  </si>
+  <si>
+    <t>too big or good</t>
+  </si>
+  <si>
+    <t>out of bounds</t>
   </si>
 </sst>
 </file>
@@ -604,7 +647,10 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top/>
+        <bottom/>
         <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -651,20 +697,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{308D8998-A54D-466C-8B5F-A0A41AE98DE1}" name="Table1" displayName="Table1" ref="A2:O22" totalsRowShown="0">
-  <autoFilter ref="A2:O22" xr:uid="{ED307D08-98E8-4842-A07F-C134845D7902}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{308D8998-A54D-466C-8B5F-A0A41AE98DE1}" name="Table1" displayName="Table1" ref="A2:P22" totalsRowShown="0">
+  <autoFilter ref="A2:P22" xr:uid="{ED307D08-98E8-4842-A07F-C134845D7902}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O22">
     <sortCondition ref="A2:A22"/>
   </sortState>
-  <tableColumns count="15">
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{3A9C98BE-0109-42FB-8BB4-10A44E726EF3}" name="Arrangement"/>
     <tableColumn id="9" xr3:uid="{B97A8DAB-F51D-41FA-B3D6-06B373BCDF3D}" name="Section"/>
     <tableColumn id="2" xr3:uid="{F2C4E4F9-BA67-4306-8E40-7C3644B78F1C}" name="Elements" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{97034C5E-0468-4431-92C4-D53DFCDEA44D}" name="XS  font-size"/>
     <tableColumn id="10" xr3:uid="{E60609C7-17F9-4FD6-9C2B-DBB60B1F4A02}" name="XS Rating" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{018873E3-3D96-4220-807B-8F6AB261B775}" name="Changes" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{018873E3-3D96-4220-807B-8F6AB261B775}" name="XS Changes" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{5B772071-8DAA-4340-BBF9-87EAF1175AFA}" name="SM  font-size"/>
-    <tableColumn id="11" xr3:uid="{60A0224E-AF8F-4BB6-B583-B5063A5B091B}" name="SM rating" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{A5250A18-ABC6-4D6C-BACA-5F4F7260986D}" name="SM Rating"/>
+    <tableColumn id="11" xr3:uid="{60A0224E-AF8F-4BB6-B583-B5063A5B091B}" name="SM Changes" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{90774B36-A071-4790-8308-284B405CDC37}" name="MD  font-size"/>
     <tableColumn id="12" xr3:uid="{0CB73393-C792-425F-BD4A-A480C0A5B74E}" name="MD rating" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{0BEA8A3F-B173-465C-9CF6-8832B4BDD53E}" name="LG  font-size"/>
@@ -974,13 +1021,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003AA83B-CD74-47A3-B603-85401DD0308B}">
-  <dimension ref="A1:O80"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,15 +1038,16 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>27</v>
       </c>
@@ -1019,8 +1067,9 @@
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="20"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -1031,43 +1080,46 @@
         <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1078,35 +1130,38 @@
         <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="N3" s="6" t="s">
+      <c r="I3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="6"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="6"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -1117,35 +1172,38 @@
         <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N4" s="8" t="s">
+      <c r="I4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -1156,35 +1214,38 @@
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="O5" s="11"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="N5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="P5" s="11"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1195,35 +1256,38 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="I6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" t="s">
         <v>71</v>
       </c>
-      <c r="G6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L6" s="6"/>
-      <c r="M6" t="s">
-        <v>73</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="O6" s="11"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K6" s="6"/>
+      <c r="L6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="P6" s="11"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -1234,35 +1298,38 @@
         <v>8</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>70</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1276,32 +1343,35 @@
         <v>3</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>62</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F8" s="11"/>
       <c r="G8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" s="6" t="s">
+      <c r="H8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="L8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="11"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="11"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1312,35 +1382,38 @@
         <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>3</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F9" s="6"/>
       <c r="G9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="N9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1351,35 +1424,38 @@
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="N10" s="6" t="s">
+      <c r="I10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="6"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>8.5</v>
       </c>
@@ -1387,38 +1463,41 @@
         <v>4</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>64</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F11" s="6"/>
       <c r="G11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="N11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -1429,35 +1508,38 @@
         <v>10</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="N12" s="6" t="s">
+      <c r="I12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="O12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" s="6"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -1468,35 +1550,38 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" s="8"/>
-      <c r="M13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N13" s="8" t="s">
+      <c r="I13" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13" s="6"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -1510,32 +1595,35 @@
         <v>3</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>63</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="F14" s="11"/>
       <c r="G14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="N14" s="6" t="s">
+      <c r="H14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="11"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14" s="11"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>12</v>
       </c>
@@ -1546,35 +1634,38 @@
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>66</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="N15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="N15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="6"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>13</v>
       </c>
@@ -1585,35 +1676,38 @@
         <v>13</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="N16" s="6" t="s">
+      <c r="I16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" s="6"/>
+      <c r="N16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="O16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>14</v>
       </c>
@@ -1624,35 +1718,38 @@
         <v>15</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="O17" s="6"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="N17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="P17" s="6"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -1663,35 +1760,38 @@
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L18" s="8"/>
-      <c r="M18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="N18" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="O18" s="8"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K18" s="8"/>
+      <c r="L18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>16</v>
       </c>
@@ -1705,30 +1805,33 @@
         <v>3</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="N19" s="6" t="s">
+      <c r="H19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" s="6"/>
+      <c r="L19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M19" s="6"/>
+      <c r="N19" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O19" s="6"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" s="6"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>17</v>
       </c>
@@ -1739,35 +1842,38 @@
         <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>3</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F20" s="6"/>
       <c r="G20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="N20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="6"/>
+      <c r="L20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20" s="6"/>
+      <c r="N20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="6"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" s="6"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>18</v>
       </c>
@@ -1778,35 +1884,38 @@
         <v>19</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="N21" s="6" t="s">
+      <c r="I21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K21" s="6"/>
+      <c r="L21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="M21" s="6"/>
+      <c r="N21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O21" s="6"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21" s="6"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>19</v>
       </c>
@@ -1817,89 +1926,92 @@
         <v>20</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>65</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F22" s="6"/>
       <c r="G22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="L22" s="8"/>
-      <c r="M22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="N22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="M22" s="8"/>
+      <c r="N22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="O22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="6"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22" s="6"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="5"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -2196,7 +2308,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="D1:P1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>